<commit_message>
added proper Lidl Pfandrückgabe handling, improved row clean up removal and adjusted kg-row handling for Kaufland
</commit_message>
<xml_diff>
--- a/src/categories.xlsx
+++ b/src/categories.xlsx
@@ -5,17 +5,29 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebi\receipt\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492B33F0-6D2E-4E8B-B45E-A2C45D9DB57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D24CEAE-478E-4BF8-9F51-47ED114913B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{9324D4E8-7F91-4615-B757-CF59BD88C93E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9324D4E8-7F91-4615-B757-CF59BD88C93E}"/>
   </bookViews>
   <sheets>
     <sheet name="Obst" sheetId="1" r:id="rId1"/>
     <sheet name="Gemüse" sheetId="2" r:id="rId2"/>
-    <sheet name="Fleischprodukte" sheetId="3" r:id="rId3"/>
+    <sheet name="Fisch" sheetId="15" r:id="rId3"/>
+    <sheet name="Fleischprodukte" sheetId="3" r:id="rId4"/>
+    <sheet name="Backwaren" sheetId="4" r:id="rId5"/>
+    <sheet name="Getränke" sheetId="5" r:id="rId6"/>
+    <sheet name="Süßwaren" sheetId="6" r:id="rId7"/>
+    <sheet name="Snacks" sheetId="7" r:id="rId8"/>
+    <sheet name="Käsestizz" sheetId="8" r:id="rId9"/>
+    <sheet name="Milch&amp;Ei" sheetId="9" r:id="rId10"/>
+    <sheet name="Grund" sheetId="10" r:id="rId11"/>
+    <sheet name="Konserve" sheetId="11" r:id="rId12"/>
+    <sheet name="Haushalt" sheetId="12" r:id="rId13"/>
+    <sheet name="Hygiene" sheetId="13" r:id="rId14"/>
+    <sheet name="Fertigprodukt" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="231">
   <si>
     <t>Apfel</t>
   </si>
@@ -545,6 +557,192 @@
   </si>
   <si>
     <t>Ingwer</t>
+  </si>
+  <si>
+    <t>Keksrolle  Vanill</t>
+  </si>
+  <si>
+    <t>Weisser Quinoa</t>
+  </si>
+  <si>
+    <t>Masken</t>
+  </si>
+  <si>
+    <t>Maxi-Duftker</t>
+  </si>
+  <si>
+    <t>Vanillezucker</t>
+  </si>
+  <si>
+    <t>Stickado Walnuss</t>
+  </si>
+  <si>
+    <t>Backpulver</t>
+  </si>
+  <si>
+    <t>Backkakao</t>
+  </si>
+  <si>
+    <t>Schokostreu, Zartbit</t>
+  </si>
+  <si>
+    <t>Kugelschr</t>
+  </si>
+  <si>
+    <t>Käseflips</t>
+  </si>
+  <si>
+    <t>Guacamole</t>
+  </si>
+  <si>
+    <t>funny frisch Orient</t>
+  </si>
+  <si>
+    <t>Spanische Pistazien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avocadoöl </t>
+  </si>
+  <si>
+    <t>Gaggli  Faden-Nestch.</t>
+  </si>
+  <si>
+    <t>Weizenmehl</t>
+  </si>
+  <si>
+    <t>Zucker</t>
+  </si>
+  <si>
+    <t>Pfanner Tee</t>
+  </si>
+  <si>
+    <t>Pfanner Weißer Tee</t>
+  </si>
+  <si>
+    <t>Pfanner grüner Tee</t>
+  </si>
+  <si>
+    <t>Haferdrink</t>
+  </si>
+  <si>
+    <t>Salatkräuter</t>
+  </si>
+  <si>
+    <t>TomateCherry</t>
+  </si>
+  <si>
+    <t>GQ Eier a.Bay. OKT</t>
+  </si>
+  <si>
+    <t>Schlagsahne</t>
+  </si>
+  <si>
+    <t>Schlagsahne 30%</t>
+  </si>
+  <si>
+    <t>Mozzarella 125g</t>
+  </si>
+  <si>
+    <t>Mozzarella</t>
+  </si>
+  <si>
+    <t>Gemüsemais</t>
+  </si>
+  <si>
+    <t>Edamer Scheiben</t>
+  </si>
+  <si>
+    <t>Gouda Scheiben</t>
+  </si>
+  <si>
+    <t>Mozarella gerieben</t>
+  </si>
+  <si>
+    <t>Milka Peanut Caramel</t>
+  </si>
+  <si>
+    <t>Fusilli</t>
+  </si>
+  <si>
+    <t>Penne Rigate</t>
+  </si>
+  <si>
+    <t>Tort. Ricotta-Spinat</t>
+  </si>
+  <si>
+    <t>Pizza Margherita 3er</t>
+  </si>
+  <si>
+    <t>Lachsseite m.H</t>
+  </si>
+  <si>
+    <t>Vernel Frisch.Morgen</t>
+  </si>
+  <si>
+    <t>Hohes C milde Orange</t>
+  </si>
+  <si>
+    <t>Traubensaft</t>
+  </si>
+  <si>
+    <t>HähnSchnitz.Curry</t>
+  </si>
+  <si>
+    <t>Tilsiter Scheiben</t>
+  </si>
+  <si>
+    <t>Emmentaler Scheiben</t>
+  </si>
+  <si>
+    <t>Fr.Eier.a.Bo.h.OKT</t>
+  </si>
+  <si>
+    <t>Schoko-Donut</t>
+  </si>
+  <si>
+    <t>Hohes C m. Frühstück</t>
+  </si>
+  <si>
+    <t>Hohes C Plus Sonnenv</t>
+  </si>
+  <si>
+    <t>Bayer.Leberk Paprika</t>
+  </si>
+  <si>
+    <t>Jogh.Mild 500g</t>
+  </si>
+  <si>
+    <t>Pommes Frites</t>
+  </si>
+  <si>
+    <t>Haferf. Kern</t>
+  </si>
+  <si>
+    <t>Crème Fraiche Kräut.</t>
+  </si>
+  <si>
+    <t>Bio Penne Rigate</t>
+  </si>
+  <si>
+    <t>MSC Fischstäbchen</t>
+  </si>
+  <si>
+    <t>Bio Spaghetti Vollk.</t>
+  </si>
+  <si>
+    <t>Pizza Hawai</t>
+  </si>
+  <si>
+    <t>Pizza Mozzarella</t>
+  </si>
+  <si>
+    <t>Pomodoro Rustica</t>
+  </si>
+  <si>
+    <t>Salsa Dip Cheese</t>
+  </si>
+  <si>
+    <t>Pflaumen dunkel</t>
   </si>
 </sst>
 </file>
@@ -934,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3664087-E083-49ED-8B01-613CC4E6D770}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +1156,7 @@
       </c>
       <c r="D1" t="str">
         <f>_xlfn.CONCAT($B$1:$B$100)</f>
-        <v>"Ananas","Ananaszylinder","Apfel","Äpfel","Apfel kg","Apfel rot","Aprikosen","Banane","Bananen","Bananen kg","Birnen","Blaubeeren","Erdbeeren","Feigen","Frucht","Granatapfel","Grapefruit","Heidelbeeren","Himbeeren","Honigmelone","Kaktusfeigen","Kirschen","Kiwi","Limetten","Mandarinen","Mango","Melone","Nektarinen","Orangen","Papaya","Passionsfrucht","Pfirsiche","Pflaumen","Plattnektarinen","Plattpfirsiche","Trauben","Trauben dunkel","Trauben hell","Trauben kernlos","Wassermelone","Weintrauben","Zitronen","Zuckermelone",</v>
+        <v>"Ananas","Ananaszylinder","Apfel","Äpfel","Apfel kg","Apfel rot","Aprikosen","Banane","Bananen","Bananen kg","Birnen","Blaubeeren","Erdbeeren","Feigen","Frucht","Granatapfel","Grapefruit","Heidelbeeren","Himbeeren","Honigmelone","Kaktusfeigen","Kirschen","Kiwi","Limetten","Mandarinen","Mango","Melone","Nektarinen","Orangen","Papaya","Passionsfrucht","Pfirsiche","Pflaumen","Plattnektarinen","Plattpfirsiche","Trauben","Trauben dunkel","Trauben hell","Trauben kernlos","Wassermelone","Weintrauben","Zitronen","Zuckermelone","Pflaumen dunkel",</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,7 +1164,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B47" si="0">CONCATENATE("""",A2,"""",",")</f>
+        <f t="shared" ref="B2:B44" si="0">CONCATENATE("""",A2,"""",",")</f>
         <v>"Ananaszylinder",</v>
       </c>
       <c r="C2" t="s">
@@ -974,7 +1172,7 @@
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("[",D1,"],")</f>
-        <v>["Ananas","Ananaszylinder","Apfel","Äpfel","Apfel kg","Apfel rot","Aprikosen","Banane","Bananen","Bananen kg","Birnen","Blaubeeren","Erdbeeren","Feigen","Frucht","Granatapfel","Grapefruit","Heidelbeeren","Himbeeren","Honigmelone","Kaktusfeigen","Kirschen","Kiwi","Limetten","Mandarinen","Mango","Melone","Nektarinen","Orangen","Papaya","Passionsfrucht","Pfirsiche","Pflaumen","Plattnektarinen","Plattpfirsiche","Trauben","Trauben dunkel","Trauben hell","Trauben kernlos","Wassermelone","Weintrauben","Zitronen","Zuckermelone",],</v>
+        <v>["Ananas","Ananaszylinder","Apfel","Äpfel","Apfel kg","Apfel rot","Aprikosen","Banane","Bananen","Bananen kg","Birnen","Blaubeeren","Erdbeeren","Feigen","Frucht","Granatapfel","Grapefruit","Heidelbeeren","Himbeeren","Honigmelone","Kaktusfeigen","Kirschen","Kiwi","Limetten","Mandarinen","Mango","Melone","Nektarinen","Orangen","Papaya","Passionsfrucht","Pfirsiche","Pflaumen","Plattnektarinen","Plattpfirsiche","Trauben","Trauben dunkel","Trauben hell","Trauben kernlos","Wassermelone","Weintrauben","Zitronen","Zuckermelone","Pflaumen dunkel",],</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,6 +1545,15 @@
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>"Zuckermelone",</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pflaumen dunkel",</v>
       </c>
     </row>
   </sheetData>
@@ -1358,12 +1565,278 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4F702F-8AA8-4D8B-828C-EA6647A73D92}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.28515625" customWidth="1"/>
+    <col min="2" max="2" width="93.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF5F1F5-DBD8-4822-B24E-57156952A254}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="102.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ECCFAD-2903-43F0-A2C8-109312580949}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D391021C-EF16-40C0-9262-C734FC1A3104}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="90.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6464F40F-957E-42FD-B2C0-FF7270C216E7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D6570A-F095-4E6A-8879-DFCB166A19DC}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="84.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3094D5C2-631B-4F8E-BF93-963ACA1DC7C4}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A52" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1858,7 @@
       </c>
       <c r="D1" t="str">
         <f>_xlfn.CONCAT($B$1:$B$100)</f>
-        <v>"Aubergine ","Avocado","Baby Spinat","Blattspinat","Blaukraut","Blumenkohl","Brokkoli","Cherrytomaten","Dattelcherrytomaten","Eisbergsalat","Erbse","Erbsen","Feldsalat","Fenchel","Grünkohl","Gurke Stk","Gurken","Ingwer","Karotten","Kartoffeln","Knoblauch","Kohlrabi","Kopfsalat","Kürbis","Lauch","Lauchzwiebeln","Mais","Mais Stk","Mangold","Mini Möhren","Miniromato","Möhren","Paprika","Paprika rot","Paprika rot, spitz","Petersilie","Pflücksalat","Pflücksalat mediter.","Radieschen","Rahmspinat","Rosenkohl","Rote Bete","Rotkohl","Rucola","Salat","Schnittlauch","Sellerie","Spargel","Spinat","Spitzpaprika","Stangenspargel","Strauchtomaten","Süßkartoffeln","TO Miniroma","Tomate","Tomaten","Weißkohl","Zucchini","Zwiebel rot","Zwiebeln",</v>
+        <v>"Aubergine ","Avocado","Baby Spinat","Blattspinat","Blaukraut","Blumenkohl","Brokkoli","Cherrytomaten","Dattelcherrytomaten","Eisbergsalat","Erbse","Erbsen","Feldsalat","Fenchel","Grünkohl","Gurke Stk","Gurken","Ingwer","Karotten","Kartoffeln","Knoblauch","Kohlrabi","Kopfsalat","Kürbis","Lauch","Lauchzwiebeln","Mais","Mais Stk","Mangold","Mini Möhren","Miniromato","Möhren","Paprika","Paprika rot","Paprika rot, spitz","Petersilie","Pflücksalat","Pflücksalat mediter.","Radieschen","Rahmspinat","Rosenkohl","Rote Bete","Rotkohl","Rucola","Salat","Schnittlauch","Sellerie","Spargel","Spinat","Spitzpaprika","Stangenspargel","Strauchtomaten","Süßkartoffeln","TO Miniroma","Tomate","Tomaten","Weißkohl","Zucchini","Zwiebel rot","Zwiebeln","Salatkräuter","TomateCherry","Eisbergsalat","Blattspinat","Dattelcherrytomaten",</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1393,7 +1866,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B60" si="0">CONCATENATE("""",A2,"""",",")</f>
+        <f t="shared" ref="B2:B65" si="0">CONCATENATE("""",A2,"""",",")</f>
         <v>"Avocado",</v>
       </c>
       <c r="C2" t="s">
@@ -1401,7 +1874,7 @@
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("[",D1,"],")</f>
-        <v>["Aubergine ","Avocado","Baby Spinat","Blattspinat","Blaukraut","Blumenkohl","Brokkoli","Cherrytomaten","Dattelcherrytomaten","Eisbergsalat","Erbse","Erbsen","Feldsalat","Fenchel","Grünkohl","Gurke Stk","Gurken","Ingwer","Karotten","Kartoffeln","Knoblauch","Kohlrabi","Kopfsalat","Kürbis","Lauch","Lauchzwiebeln","Mais","Mais Stk","Mangold","Mini Möhren","Miniromato","Möhren","Paprika","Paprika rot","Paprika rot, spitz","Petersilie","Pflücksalat","Pflücksalat mediter.","Radieschen","Rahmspinat","Rosenkohl","Rote Bete","Rotkohl","Rucola","Salat","Schnittlauch","Sellerie","Spargel","Spinat","Spitzpaprika","Stangenspargel","Strauchtomaten","Süßkartoffeln","TO Miniroma","Tomate","Tomaten","Weißkohl","Zucchini","Zwiebel rot","Zwiebeln",],</v>
+        <v>["Aubergine ","Avocado","Baby Spinat","Blattspinat","Blaukraut","Blumenkohl","Brokkoli","Cherrytomaten","Dattelcherrytomaten","Eisbergsalat","Erbse","Erbsen","Feldsalat","Fenchel","Grünkohl","Gurke Stk","Gurken","Ingwer","Karotten","Kartoffeln","Knoblauch","Kohlrabi","Kopfsalat","Kürbis","Lauch","Lauchzwiebeln","Mais","Mais Stk","Mangold","Mini Möhren","Miniromato","Möhren","Paprika","Paprika rot","Paprika rot, spitz","Petersilie","Pflücksalat","Pflücksalat mediter.","Radieschen","Rahmspinat","Rosenkohl","Rote Bete","Rotkohl","Rucola","Salat","Schnittlauch","Sellerie","Spargel","Spinat","Spitzpaprika","Stangenspargel","Strauchtomaten","Süßkartoffeln","TO Miniroma","Tomate","Tomaten","Weißkohl","Zucchini","Zwiebel rot","Zwiebeln","Salatkräuter","TomateCherry","Eisbergsalat","Blattspinat","Dattelcherrytomaten",],</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,6 +2400,51 @@
       <c r="B60" t="str">
         <f t="shared" si="0"/>
         <v>"Zwiebeln",</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>191</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>"Salatkräuter",</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>"TomateCherry",</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>"Eisbergsalat",</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>"Blattspinat",</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>"Dattelcherrytomaten",</v>
       </c>
     </row>
   </sheetData>
@@ -1939,11 +2457,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFF400C-1494-476F-AC4C-EBF327110932}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFE4810-61E7-49F5-AF43-49F5B6875649}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A58" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,7 +2511,7 @@
       </c>
       <c r="D1" t="str">
         <f>_xlfn.CONCAT($B$1:$B$100)</f>
-        <v>"Aoste Stickado &amp; Brot","Bayer. Leberk","Bayerischer Leberkäse","Cevapcici","Chicken","Chicken Nuggets","Cordon Bleu","Gefl. Lyoner","Gefl. Lyoner","Gefl. Mortadella","Geflügelleberwurst","Geflügel-Mortadella","Geschnet.","Geschnetzeltes","Grillschinken","Gutsleberwurst","Gyros","Hä.Geschnetz.","Hackfleisch","Hackfleisch gemischt","Haenchenbrust","Hähn.-Geschnetzeltes","Hähnchenbr. hauchd.","Hänchen","Hänchen Schnitzel","Hänchenbr.","Hänchenbrust","Huhn","Hünchenbrust","Karli Knusper Dinos","Katenschinken","Katenschinken Würfel","Leberkäse","Leberwurst","Lyoner","Mortadella","P.Hackfleisch","Pfefferbeißer","Pommersche","Puten Mini-Steaks","Puten-Geschnetzeltes","Puten-Mini-Steaks","Putenschni.","Putenschnitzel","Rinder Cevapcici","Rinderhackfleisch","Roast Chicken","Royal Hänchenbrust","Rü. Schnitzel veg.","Rü.Pomm.Schnitll.","Rü.Salami Peperoni","Rüg. Schinkensp. Pf.","Rügenwalder","Salami","Salami Sticks","Schinken","Schinkenwürfel","Schnitzel","Steak","Stickado","Stickado Hähnchen","Truthahnbrust","Truthahnschinken","Wurst/Schinken",</v>
+        <v>"Aoste Stickado &amp; Brot","Bayer. Leberk","Bayerischer Leberkäse","Cevapcici","Chicken","Chicken Nuggets","Cordon Bleu","Gefl. Lyoner","Gefl. Lyoner","Gefl. Mortadella","Geflügelleberwurst","Geflügel-Mortadella","Geschnet.","Geschnetzeltes","Grillschinken","Gutsleberwurst","Gyros","Hä.Geschnetz.","Hackfleisch","Hackfleisch gemischt","Haenchenbrust","Hähn.-Geschnetzeltes","Hähnchenbr. hauchd.","Hänchen","Hänchen Schnitzel","Hänchenbr.","Hänchenbrust","Huhn","Hünchenbrust","Karli Knusper Dinos","Katenschinken","Katenschinken Würfel","Leberkäse","Leberwurst","Lyoner","Mortadella","P.Hackfleisch","Pfefferbeißer","Pommersche","Puten Mini-Steaks","Puten-Geschnetzeltes","Puten-Mini-Steaks","Putenschni.","Putenschnitzel","Rinder Cevapcici","Rinderhackfleisch","Roast Chicken","Royal Hänchenbrust","Rü. Schnitzel veg.","Rü.Pomm.Schnitll.","Rü.Salami Peperoni","Rüg. Schinkensp. Pf.","Rügenwalder","Salami","Salami Sticks","Schinken","Schinkenwürfel","Schnitzel","Steak","Stickado","Stickado Hähnchen","Truthahnbrust","Truthahnschinken","Wurst/Schinken","Stickado Walnuss","HähnSchnitz.Curry","Bayer.Leberk Paprika",</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1973,7 +2519,7 @@
         <v>145</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B64" si="0">CONCATENATE("""",A2,"""",",")</f>
+        <f t="shared" ref="B2:B67" si="0">CONCATENATE("""",A2,"""",",")</f>
         <v>"Bayer. Leberk",</v>
       </c>
       <c r="C2" t="s">
@@ -1981,7 +2527,7 @@
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("[",D1,"],")</f>
-        <v>["Aoste Stickado &amp; Brot","Bayer. Leberk","Bayerischer Leberkäse","Cevapcici","Chicken","Chicken Nuggets","Cordon Bleu","Gefl. Lyoner","Gefl. Lyoner","Gefl. Mortadella","Geflügelleberwurst","Geflügel-Mortadella","Geschnet.","Geschnetzeltes","Grillschinken","Gutsleberwurst","Gyros","Hä.Geschnetz.","Hackfleisch","Hackfleisch gemischt","Haenchenbrust","Hähn.-Geschnetzeltes","Hähnchenbr. hauchd.","Hänchen","Hänchen Schnitzel","Hänchenbr.","Hänchenbrust","Huhn","Hünchenbrust","Karli Knusper Dinos","Katenschinken","Katenschinken Würfel","Leberkäse","Leberwurst","Lyoner","Mortadella","P.Hackfleisch","Pfefferbeißer","Pommersche","Puten Mini-Steaks","Puten-Geschnetzeltes","Puten-Mini-Steaks","Putenschni.","Putenschnitzel","Rinder Cevapcici","Rinderhackfleisch","Roast Chicken","Royal Hänchenbrust","Rü. Schnitzel veg.","Rü.Pomm.Schnitll.","Rü.Salami Peperoni","Rüg. Schinkensp. Pf.","Rügenwalder","Salami","Salami Sticks","Schinken","Schinkenwürfel","Schnitzel","Steak","Stickado","Stickado Hähnchen","Truthahnbrust","Truthahnschinken","Wurst/Schinken",],</v>
+        <v>["Aoste Stickado &amp; Brot","Bayer. Leberk","Bayerischer Leberkäse","Cevapcici","Chicken","Chicken Nuggets","Cordon Bleu","Gefl. Lyoner","Gefl. Lyoner","Gefl. Mortadella","Geflügelleberwurst","Geflügel-Mortadella","Geschnet.","Geschnetzeltes","Grillschinken","Gutsleberwurst","Gyros","Hä.Geschnetz.","Hackfleisch","Hackfleisch gemischt","Haenchenbrust","Hähn.-Geschnetzeltes","Hähnchenbr. hauchd.","Hänchen","Hänchen Schnitzel","Hänchenbr.","Hänchenbrust","Huhn","Hünchenbrust","Karli Knusper Dinos","Katenschinken","Katenschinken Würfel","Leberkäse","Leberwurst","Lyoner","Mortadella","P.Hackfleisch","Pfefferbeißer","Pommersche","Puten Mini-Steaks","Puten-Geschnetzeltes","Puten-Mini-Steaks","Putenschni.","Putenschnitzel","Rinder Cevapcici","Rinderhackfleisch","Roast Chicken","Royal Hänchenbrust","Rü. Schnitzel veg.","Rü.Pomm.Schnitll.","Rü.Salami Peperoni","Rüg. Schinkensp. Pf.","Rügenwalder","Salami","Salami Sticks","Schinken","Schinkenwürfel","Schnitzel","Steak","Stickado","Stickado Hähnchen","Truthahnbrust","Truthahnschinken","Wurst/Schinken","Stickado Walnuss","HähnSchnitz.Curry","Bayer.Leberk Paprika",],</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2543,6 +3089,33 @@
       <c r="B64" t="str">
         <f t="shared" si="0"/>
         <v>"Wurst/Schinken",</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>"Stickado Walnuss",</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>"HähnSchnitz.Curry",</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="0"/>
+        <v>"Bayer.Leberk Paprika",</v>
       </c>
     </row>
   </sheetData>
@@ -2552,4 +3125,206 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA11805D-E507-4C2A-9E2F-386B2CEEB433}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64" customWidth="1"/>
+    <col min="2" max="2" width="83" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B464F9C-5F5D-47D6-93BB-E14294E72AC7}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77B1EA0-7C6F-4577-B387-458AC9F459CC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF88087-48C6-4700-8786-3D611FC395D6}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="71.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D21FAC2-72A4-4722-9547-A3EA512419AA}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>